<commit_message>
Tested the Data gather module
</commit_message>
<xml_diff>
--- a/Input_from_client.xlsx
+++ b/Input_from_client.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7530"/>
+    <workbookView windowWidth="20490" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="Truck_Route_line" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Truck_Route_line!$A$1:$G$49</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -133,7 +146,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>

</xml_diff>